<commit_message>
Use `keywords` as a kwarg when creating StatefulBook to set the search terms column heading. Defaults to "item".
</commit_message>
<xml_diff>
--- a/examples/books_to_scrape/book_titles.xlsx
+++ b/examples/books_to_scrape/book_titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjord\repos\transistor\examples\books_to_scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D571C74A-005E-4E4E-BCCA-EE6A073491DC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26487216-26EA-4C4D-9D36-4DD56E708F10}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11685" windowHeight="4148" xr2:uid="{A981794D-1504-4842-AF12-31D3D191C2DD}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>item</t>
-  </si>
-  <si>
     <t>Soumission</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Two Summers</t>
+  </si>
+  <si>
+    <t>titles</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -476,107 +476,107 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>